<commit_message>
design vistds plot v1
</commit_message>
<xml_diff>
--- a/bshe/VIS_opf/ieee39_vis_tds.xlsx
+++ b/bshe/VIS_opf/ieee39_vis_tds.xlsx
@@ -2558,11 +2558,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6">
-      <c r="N6" t="str">
-        <v>ß</v>
-      </c>
-    </row>
     <row r="7">
       <c r="U7" t="str">
         <v/>
@@ -4349,7 +4344,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4542,7 +4537,7 @@
         <v>SG_2</v>
       </c>
       <c r="E7" t="str">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F7" t="str">
         <v>0.002</v>
@@ -4557,9 +4552,125 @@
         <v>0.001</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>6</v>
+      </c>
+      <c r="B8" t="str">
+        <v>1</v>
+      </c>
+      <c r="C8" t="str">
+        <v>BusROCOF_7</v>
+      </c>
+      <c r="D8" t="str">
+        <v>SG_3</v>
+      </c>
+      <c r="E8" t="str">
+        <v>33</v>
+      </c>
+      <c r="F8" t="str">
+        <v>0.002</v>
+      </c>
+      <c r="G8" t="str">
+        <v>0.02</v>
+      </c>
+      <c r="H8" t="str">
+        <v>60</v>
+      </c>
+      <c r="I8" t="str">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>7</v>
+      </c>
+      <c r="B9" t="str">
+        <v>1</v>
+      </c>
+      <c r="C9" t="str">
+        <v>BusROCOF_8</v>
+      </c>
+      <c r="D9" t="str">
+        <v>SG_4</v>
+      </c>
+      <c r="E9" t="str">
+        <v>34</v>
+      </c>
+      <c r="F9" t="str">
+        <v>0.002</v>
+      </c>
+      <c r="G9" t="str">
+        <v>0.02</v>
+      </c>
+      <c r="H9" t="str">
+        <v>60</v>
+      </c>
+      <c r="I9" t="str">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>8</v>
+      </c>
+      <c r="B10" t="str">
+        <v>1</v>
+      </c>
+      <c r="C10" t="str">
+        <v>BusROCOF_9</v>
+      </c>
+      <c r="D10" t="str">
+        <v>SG_5</v>
+      </c>
+      <c r="E10" t="str">
+        <v>36</v>
+      </c>
+      <c r="F10" t="str">
+        <v>0.002</v>
+      </c>
+      <c r="G10" t="str">
+        <v>0.02</v>
+      </c>
+      <c r="H10" t="str">
+        <v>60</v>
+      </c>
+      <c r="I10" t="str">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>9</v>
+      </c>
+      <c r="B11" t="str">
+        <v>1</v>
+      </c>
+      <c r="C11" t="str">
+        <v>BusROCOF_10</v>
+      </c>
+      <c r="D11" t="str">
+        <v>SG_6</v>
+      </c>
+      <c r="E11" t="str">
+        <v>39</v>
+      </c>
+      <c r="F11" t="str">
+        <v>0.002</v>
+      </c>
+      <c r="G11" t="str">
+        <v>0.02</v>
+      </c>
+      <c r="H11" t="str">
+        <v>60</v>
+      </c>
+      <c r="I11" t="str">
+        <v>0.001</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I11"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>